<commit_message>
add sheet2 in result.xlx
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/科研/Research/Code/COOP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFD2117-F4C9-8945-B395-96FBF6282E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DD78F4-4CF4-0542-A2F3-61B2B3A35786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="imcls_fewshot" sheetId="1" r:id="rId1"/>
+    <sheet name="imcls_fewshot (ours)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -83,8 +84,53 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="B24" authorId="0" shapeId="0" xr:uid="{E3638D09-2525-D946-8E71-6828A8C0653D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>======
+ID#AAAASc0lCi4
+Implementation Details    (2021-12-06 01:16:10)
+1. Extract ResNet50 CLIP features (visual encoder with dim=1024)
+2. 1/2/4/8/16-shot training corresponds to 1/2/4/4/4-shot for validation set.
+3. Since no validation set for ImageNet, we make use of hyperparam of Caltech-101 for ImageNet.
+4. Every experiment runs 3 seeds to compute mean/std.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M28" authorId="0" shapeId="0" xr:uid="{7230E8E6-1936-694F-851B-D7C4106B707D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>======
+ID#AAAASc0lCiw
+    (2021-12-06 01:16:10)
+lambda around 0.001</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="40">
   <si>
     <t>Index</t>
   </si>
@@ -321,7 +367,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -329,11 +375,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -383,6 +444,26 @@
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -603,9 +684,9 @@
   </sheetPr>
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G32" sqref="G32"/>
+      <selection pane="topRight" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -1766,6 +1847,2297 @@
         <v>73.72</v>
       </c>
       <c r="M28" s="18">
+        <v>55.87</v>
+      </c>
+      <c r="N28" s="8"/>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A29" s="5"/>
+      <c r="N29" s="8"/>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A30" s="5"/>
+      <c r="N30" s="8"/>
+    </row>
+    <row r="31" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A31" s="5"/>
+      <c r="N31" s="8"/>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A32" s="5"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="8"/>
+    </row>
+    <row r="33" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A33" s="5"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="8"/>
+    </row>
+    <row r="34" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A34" s="5"/>
+      <c r="N34" s="22"/>
+    </row>
+    <row r="35" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A35" s="5"/>
+      <c r="N35" s="22"/>
+    </row>
+    <row r="36" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A36" s="5"/>
+      <c r="N36" s="22"/>
+    </row>
+    <row r="37" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A37" s="5"/>
+      <c r="N37" s="22"/>
+    </row>
+    <row r="38" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A38" s="5"/>
+      <c r="N38" s="22"/>
+    </row>
+    <row r="39" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A39" s="5"/>
+      <c r="N39" s="22"/>
+    </row>
+    <row r="40" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A40" s="5"/>
+      <c r="N40" s="8"/>
+    </row>
+    <row r="41" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A41" s="5"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
+      <c r="L41" s="24"/>
+      <c r="M41" s="24"/>
+      <c r="N41" s="8"/>
+    </row>
+    <row r="42" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A42" s="5"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="22"/>
+    </row>
+    <row r="43" spans="1:14" ht="15.75" customHeight="1">
+      <c r="N43" s="8"/>
+    </row>
+    <row r="44" spans="1:14" ht="15.75" customHeight="1">
+      <c r="N44" s="8"/>
+    </row>
+    <row r="45" spans="1:14" ht="15.75" customHeight="1">
+      <c r="N45" s="8"/>
+    </row>
+    <row r="46" spans="1:14" ht="15.75" customHeight="1">
+      <c r="N46" s="8"/>
+    </row>
+    <row r="47" spans="1:14" ht="15.75" customHeight="1">
+      <c r="N47" s="8"/>
+    </row>
+    <row r="48" spans="1:14" ht="15.75" customHeight="1">
+      <c r="N48" s="8"/>
+    </row>
+    <row r="49" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N49" s="8"/>
+    </row>
+    <row r="50" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N50" s="8"/>
+    </row>
+    <row r="51" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N51" s="8"/>
+    </row>
+    <row r="52" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N52" s="8"/>
+    </row>
+    <row r="53" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N53" s="8"/>
+    </row>
+    <row r="54" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N54" s="8"/>
+    </row>
+    <row r="55" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N55" s="8"/>
+    </row>
+    <row r="56" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N56" s="8"/>
+    </row>
+    <row r="57" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N57" s="8"/>
+    </row>
+    <row r="58" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N58" s="8"/>
+    </row>
+    <row r="59" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N59" s="8"/>
+    </row>
+    <row r="60" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N60" s="8"/>
+    </row>
+    <row r="61" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N61" s="8"/>
+    </row>
+    <row r="62" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N62" s="8"/>
+    </row>
+    <row r="63" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N63" s="8"/>
+    </row>
+    <row r="64" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N64" s="8"/>
+    </row>
+    <row r="65" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N65" s="8"/>
+    </row>
+    <row r="66" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N66" s="8"/>
+    </row>
+    <row r="67" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N67" s="8"/>
+    </row>
+    <row r="68" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N68" s="8"/>
+    </row>
+    <row r="69" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N69" s="8"/>
+    </row>
+    <row r="70" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N70" s="8"/>
+    </row>
+    <row r="71" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N71" s="8"/>
+    </row>
+    <row r="72" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N72" s="8"/>
+    </row>
+    <row r="73" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N73" s="8"/>
+    </row>
+    <row r="74" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N74" s="8"/>
+    </row>
+    <row r="75" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N75" s="8"/>
+    </row>
+    <row r="76" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N76" s="8"/>
+    </row>
+    <row r="77" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N77" s="8"/>
+    </row>
+    <row r="78" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N78" s="8"/>
+    </row>
+    <row r="79" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N79" s="8"/>
+    </row>
+    <row r="80" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N80" s="8"/>
+    </row>
+    <row r="81" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N81" s="8"/>
+    </row>
+    <row r="82" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N82" s="8"/>
+    </row>
+    <row r="83" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N83" s="8"/>
+    </row>
+    <row r="84" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N84" s="8"/>
+    </row>
+    <row r="85" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N85" s="8"/>
+    </row>
+    <row r="86" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N86" s="8"/>
+    </row>
+    <row r="87" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N87" s="8"/>
+    </row>
+    <row r="88" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N88" s="8"/>
+    </row>
+    <row r="89" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N89" s="8"/>
+    </row>
+    <row r="90" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N90" s="8"/>
+    </row>
+    <row r="91" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N91" s="8"/>
+    </row>
+    <row r="92" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N92" s="8"/>
+    </row>
+    <row r="93" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N93" s="8"/>
+    </row>
+    <row r="94" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N94" s="8"/>
+    </row>
+    <row r="95" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N95" s="8"/>
+    </row>
+    <row r="96" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N96" s="8"/>
+    </row>
+    <row r="97" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N97" s="8"/>
+    </row>
+    <row r="98" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N98" s="8"/>
+    </row>
+    <row r="99" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N99" s="8"/>
+    </row>
+    <row r="100" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N100" s="8"/>
+    </row>
+    <row r="101" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N101" s="8"/>
+    </row>
+    <row r="102" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N102" s="8"/>
+    </row>
+    <row r="103" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N103" s="8"/>
+    </row>
+    <row r="104" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N104" s="8"/>
+    </row>
+    <row r="105" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N105" s="8"/>
+    </row>
+    <row r="106" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N106" s="8"/>
+    </row>
+    <row r="107" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N107" s="8"/>
+    </row>
+    <row r="108" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N108" s="8"/>
+    </row>
+    <row r="109" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N109" s="8"/>
+    </row>
+    <row r="110" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N110" s="8"/>
+    </row>
+    <row r="111" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N111" s="8"/>
+    </row>
+    <row r="112" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N112" s="8"/>
+    </row>
+    <row r="113" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N113" s="8"/>
+    </row>
+    <row r="114" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N114" s="8"/>
+    </row>
+    <row r="115" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N115" s="8"/>
+    </row>
+    <row r="116" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N116" s="8"/>
+    </row>
+    <row r="117" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N117" s="8"/>
+    </row>
+    <row r="118" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N118" s="8"/>
+    </row>
+    <row r="119" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N119" s="8"/>
+    </row>
+    <row r="120" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N120" s="8"/>
+    </row>
+    <row r="121" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N121" s="8"/>
+    </row>
+    <row r="122" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N122" s="8"/>
+    </row>
+    <row r="123" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N123" s="8"/>
+    </row>
+    <row r="124" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N124" s="8"/>
+    </row>
+    <row r="125" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N125" s="8"/>
+    </row>
+    <row r="126" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N126" s="8"/>
+    </row>
+    <row r="127" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N127" s="8"/>
+    </row>
+    <row r="128" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N128" s="8"/>
+    </row>
+    <row r="129" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N129" s="8"/>
+    </row>
+    <row r="130" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N130" s="8"/>
+    </row>
+    <row r="131" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N131" s="8"/>
+    </row>
+    <row r="132" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N132" s="8"/>
+    </row>
+    <row r="133" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N133" s="8"/>
+    </row>
+    <row r="134" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N134" s="8"/>
+    </row>
+    <row r="135" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N135" s="8"/>
+    </row>
+    <row r="136" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N136" s="8"/>
+    </row>
+    <row r="137" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N137" s="8"/>
+    </row>
+    <row r="138" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N138" s="8"/>
+    </row>
+    <row r="139" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N139" s="8"/>
+    </row>
+    <row r="140" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N140" s="8"/>
+    </row>
+    <row r="141" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N141" s="8"/>
+    </row>
+    <row r="142" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N142" s="8"/>
+    </row>
+    <row r="143" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N143" s="8"/>
+    </row>
+    <row r="144" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N144" s="8"/>
+    </row>
+    <row r="145" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N145" s="8"/>
+    </row>
+    <row r="146" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N146" s="8"/>
+    </row>
+    <row r="147" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N147" s="8"/>
+    </row>
+    <row r="148" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N148" s="8"/>
+    </row>
+    <row r="149" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N149" s="8"/>
+    </row>
+    <row r="150" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N150" s="8"/>
+    </row>
+    <row r="151" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N151" s="8"/>
+    </row>
+    <row r="152" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N152" s="8"/>
+    </row>
+    <row r="153" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N153" s="8"/>
+    </row>
+    <row r="154" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N154" s="8"/>
+    </row>
+    <row r="155" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N155" s="8"/>
+    </row>
+    <row r="156" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N156" s="8"/>
+    </row>
+    <row r="157" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N157" s="8"/>
+    </row>
+    <row r="158" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N158" s="8"/>
+    </row>
+    <row r="159" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N159" s="8"/>
+    </row>
+    <row r="160" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N160" s="8"/>
+    </row>
+    <row r="161" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N161" s="8"/>
+    </row>
+    <row r="162" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N162" s="8"/>
+    </row>
+    <row r="163" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N163" s="8"/>
+    </row>
+    <row r="164" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N164" s="8"/>
+    </row>
+    <row r="165" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N165" s="8"/>
+    </row>
+    <row r="166" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N166" s="8"/>
+    </row>
+    <row r="167" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N167" s="8"/>
+    </row>
+    <row r="168" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N168" s="8"/>
+    </row>
+    <row r="169" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N169" s="8"/>
+    </row>
+    <row r="170" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N170" s="8"/>
+    </row>
+    <row r="171" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N171" s="8"/>
+    </row>
+    <row r="172" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N172" s="8"/>
+    </row>
+    <row r="173" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N173" s="8"/>
+    </row>
+    <row r="174" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N174" s="8"/>
+    </row>
+    <row r="175" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N175" s="8"/>
+    </row>
+    <row r="176" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N176" s="8"/>
+    </row>
+    <row r="177" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N177" s="8"/>
+    </row>
+    <row r="178" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N178" s="8"/>
+    </row>
+    <row r="179" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N179" s="8"/>
+    </row>
+    <row r="180" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N180" s="8"/>
+    </row>
+    <row r="181" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N181" s="8"/>
+    </row>
+    <row r="182" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N182" s="8"/>
+    </row>
+    <row r="183" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N183" s="8"/>
+    </row>
+    <row r="184" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N184" s="8"/>
+    </row>
+    <row r="185" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N185" s="8"/>
+    </row>
+    <row r="186" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N186" s="8"/>
+    </row>
+    <row r="187" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N187" s="8"/>
+    </row>
+    <row r="188" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N188" s="8"/>
+    </row>
+    <row r="189" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N189" s="8"/>
+    </row>
+    <row r="190" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N190" s="8"/>
+    </row>
+    <row r="191" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N191" s="8"/>
+    </row>
+    <row r="192" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N192" s="8"/>
+    </row>
+    <row r="193" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N193" s="8"/>
+    </row>
+    <row r="194" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N194" s="8"/>
+    </row>
+    <row r="195" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N195" s="8"/>
+    </row>
+    <row r="196" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N196" s="8"/>
+    </row>
+    <row r="197" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N197" s="8"/>
+    </row>
+    <row r="198" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N198" s="8"/>
+    </row>
+    <row r="199" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N199" s="8"/>
+    </row>
+    <row r="200" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N200" s="8"/>
+    </row>
+    <row r="201" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N201" s="8"/>
+    </row>
+    <row r="202" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N202" s="8"/>
+    </row>
+    <row r="203" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N203" s="8"/>
+    </row>
+    <row r="204" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N204" s="8"/>
+    </row>
+    <row r="205" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N205" s="8"/>
+    </row>
+    <row r="206" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N206" s="8"/>
+    </row>
+    <row r="207" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N207" s="8"/>
+    </row>
+    <row r="208" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N208" s="8"/>
+    </row>
+    <row r="209" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N209" s="8"/>
+    </row>
+    <row r="210" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N210" s="8"/>
+    </row>
+    <row r="211" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N211" s="8"/>
+    </row>
+    <row r="212" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N212" s="8"/>
+    </row>
+    <row r="213" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N213" s="8"/>
+    </row>
+    <row r="214" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N214" s="8"/>
+    </row>
+    <row r="215" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N215" s="8"/>
+    </row>
+    <row r="216" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N216" s="8"/>
+    </row>
+    <row r="217" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N217" s="8"/>
+    </row>
+    <row r="218" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N218" s="8"/>
+    </row>
+    <row r="219" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N219" s="8"/>
+    </row>
+    <row r="220" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N220" s="8"/>
+    </row>
+    <row r="221" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N221" s="8"/>
+    </row>
+    <row r="222" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N222" s="8"/>
+    </row>
+    <row r="223" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N223" s="8"/>
+    </row>
+    <row r="224" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N224" s="8"/>
+    </row>
+    <row r="225" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N225" s="8"/>
+    </row>
+    <row r="226" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N226" s="8"/>
+    </row>
+    <row r="227" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N227" s="8"/>
+    </row>
+    <row r="228" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N228" s="8"/>
+    </row>
+    <row r="229" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N229" s="8"/>
+    </row>
+    <row r="230" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N230" s="8"/>
+    </row>
+    <row r="231" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N231" s="8"/>
+    </row>
+    <row r="232" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N232" s="8"/>
+    </row>
+    <row r="233" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N233" s="8"/>
+    </row>
+    <row r="234" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N234" s="8"/>
+    </row>
+    <row r="235" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N235" s="8"/>
+    </row>
+    <row r="236" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N236" s="8"/>
+    </row>
+    <row r="237" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N237" s="8"/>
+    </row>
+    <row r="238" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N238" s="8"/>
+    </row>
+    <row r="239" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N239" s="8"/>
+    </row>
+    <row r="240" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N240" s="8"/>
+    </row>
+    <row r="241" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N241" s="8"/>
+    </row>
+    <row r="242" spans="14:14" ht="15.75" customHeight="1">
+      <c r="N242" s="8"/>
+    </row>
+    <row r="243" spans="14:14" ht="15.75" customHeight="1"/>
+    <row r="244" spans="14:14" ht="15.75" customHeight="1"/>
+    <row r="245" spans="14:14" ht="15.75" customHeight="1"/>
+    <row r="246" spans="14:14" ht="15.75" customHeight="1"/>
+    <row r="247" spans="14:14" ht="15.75" customHeight="1"/>
+    <row r="248" spans="14:14" ht="15.75" customHeight="1"/>
+    <row r="249" spans="14:14" ht="15.75" customHeight="1"/>
+    <row r="250" spans="14:14" ht="15.75" customHeight="1"/>
+    <row r="251" spans="14:14" ht="15.75" customHeight="1"/>
+    <row r="252" spans="14:14" ht="15.75" customHeight="1"/>
+    <row r="253" spans="14:14" ht="15.75" customHeight="1"/>
+    <row r="254" spans="14:14" ht="15.75" customHeight="1"/>
+    <row r="255" spans="14:14" ht="15.75" customHeight="1"/>
+    <row r="256" spans="14:14" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239EA370-7DDE-B645-A2FD-686727A9FFE0}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:N1000"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="40.5" style="4" customWidth="1"/>
+    <col min="3" max="6" width="14.5" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="14.5" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A2" s="5">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="7">
+        <v>85.77</v>
+      </c>
+      <c r="D2" s="7">
+        <v>66.14</v>
+      </c>
+      <c r="E2" s="7">
+        <v>17.28</v>
+      </c>
+      <c r="F2" s="7">
+        <v>42.32</v>
+      </c>
+      <c r="G2" s="7">
+        <v>37.56</v>
+      </c>
+      <c r="H2" s="7">
+        <v>55.61</v>
+      </c>
+      <c r="I2" s="7">
+        <v>77.31</v>
+      </c>
+      <c r="J2" s="7">
+        <v>58.52</v>
+      </c>
+      <c r="K2" s="7">
+        <v>86.29</v>
+      </c>
+      <c r="L2" s="7">
+        <v>61.46</v>
+      </c>
+      <c r="M2" s="7">
+        <v>58.18</v>
+      </c>
+      <c r="N2" s="8"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="8"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="8"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="8"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="8"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="26">
+        <v>87.01</v>
+      </c>
+      <c r="D8" s="26">
+        <v>94.51</v>
+      </c>
+      <c r="E8" s="26">
+        <v>31.26</v>
+      </c>
+      <c r="F8" s="26">
+        <v>63.58</v>
+      </c>
+      <c r="G8" s="26">
+        <v>83.53</v>
+      </c>
+      <c r="H8" s="26">
+        <v>73.36</v>
+      </c>
+      <c r="I8" s="26">
+        <v>74.67</v>
+      </c>
+      <c r="J8" s="26">
+        <v>69.260000000000005</v>
+      </c>
+      <c r="K8" s="26">
+        <v>91.83</v>
+      </c>
+      <c r="L8" s="26">
+        <v>75.709999999999994</v>
+      </c>
+      <c r="M8" s="26">
+        <v>62.95</v>
+      </c>
+      <c r="N8" s="8"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="8"/>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A10" s="5">
+        <v>8</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="8"/>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A11" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="8"/>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="8"/>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A13" s="5">
+        <v>11</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="28">
+        <v>86.16</v>
+      </c>
+      <c r="D13" s="28">
+        <v>94.8</v>
+      </c>
+      <c r="E13" s="28">
+        <v>32.29</v>
+      </c>
+      <c r="F13" s="28">
+        <v>63.16</v>
+      </c>
+      <c r="G13" s="28">
+        <v>83.55</v>
+      </c>
+      <c r="H13" s="28">
+        <v>73.27</v>
+      </c>
+      <c r="I13" s="28">
+        <v>74.459999999999994</v>
+      </c>
+      <c r="J13" s="28">
+        <v>69.12</v>
+      </c>
+      <c r="K13" s="28">
+        <v>91.62</v>
+      </c>
+      <c r="L13" s="28">
+        <v>75.290000000000006</v>
+      </c>
+      <c r="M13" s="28">
+        <v>63.08</v>
+      </c>
+      <c r="N13" s="8"/>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A14" s="5">
+        <v>12</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="8"/>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A15" s="5">
+        <v>13</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="8"/>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A16" s="5">
+        <v>14</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="8"/>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A17" s="5">
+        <v>15</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="8"/>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A18" s="5">
+        <v>16</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="28">
+        <v>86.16</v>
+      </c>
+      <c r="D18" s="28">
+        <v>94.8</v>
+      </c>
+      <c r="E18" s="28">
+        <v>32.29</v>
+      </c>
+      <c r="F18" s="28">
+        <v>63.16</v>
+      </c>
+      <c r="G18" s="28">
+        <v>83.55</v>
+      </c>
+      <c r="H18" s="28">
+        <v>73.27</v>
+      </c>
+      <c r="I18" s="28">
+        <v>74.459999999999994</v>
+      </c>
+      <c r="J18" s="28">
+        <v>69.12</v>
+      </c>
+      <c r="K18" s="28">
+        <v>91.62</v>
+      </c>
+      <c r="L18" s="28">
+        <v>75.290000000000006</v>
+      </c>
+      <c r="M18" s="28">
+        <v>63.08</v>
+      </c>
+      <c r="N18" s="8"/>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A19" s="5">
+        <v>17</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="8"/>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A20" s="5">
+        <v>18</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="8"/>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A21" s="5">
+        <v>19</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="8"/>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A22" s="5">
+        <v>20</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="8"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A23" s="5">
+        <v>21</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="32">
+        <v>80.87</v>
+      </c>
+      <c r="D23" s="32">
+        <v>95.52</v>
+      </c>
+      <c r="E23" s="32">
+        <v>37.479999999999997</v>
+      </c>
+      <c r="F23" s="32">
+        <v>62.57</v>
+      </c>
+      <c r="G23" s="32">
+        <v>84.87</v>
+      </c>
+      <c r="H23" s="32">
+        <v>72.319999999999993</v>
+      </c>
+      <c r="I23" s="32">
+        <v>70.040000000000006</v>
+      </c>
+      <c r="J23" s="32">
+        <v>63.76</v>
+      </c>
+      <c r="K23" s="32">
+        <v>90.57</v>
+      </c>
+      <c r="L23" s="32">
+        <v>73.349999999999994</v>
+      </c>
+      <c r="M23" s="32">
+        <v>54.65</v>
+      </c>
+      <c r="N23" s="8"/>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A24" s="5">
+        <v>22</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="34">
+        <v>30.14</v>
+      </c>
+      <c r="D24" s="34">
+        <v>58.07</v>
+      </c>
+      <c r="E24" s="34">
+        <v>12.89</v>
+      </c>
+      <c r="F24" s="34">
+        <v>29.59</v>
+      </c>
+      <c r="G24" s="34">
+        <v>51</v>
+      </c>
+      <c r="H24" s="34">
+        <v>24.64</v>
+      </c>
+      <c r="I24" s="34">
+        <v>30.13</v>
+      </c>
+      <c r="J24" s="34">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="K24" s="34">
+        <v>70.62</v>
+      </c>
+      <c r="L24" s="34">
+        <v>41.43</v>
+      </c>
+      <c r="M24" s="34">
+        <v>22.07</v>
+      </c>
+      <c r="N24" s="8"/>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A25" s="5">
+        <v>23</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="34">
+        <v>43.47</v>
+      </c>
+      <c r="D25" s="34">
+        <v>73.349999999999994</v>
+      </c>
+      <c r="E25" s="34">
+        <v>17.850000000000001</v>
+      </c>
+      <c r="F25" s="34">
+        <v>39.479999999999997</v>
+      </c>
+      <c r="G25" s="34">
+        <v>61.58</v>
+      </c>
+      <c r="H25" s="34">
+        <v>36.53</v>
+      </c>
+      <c r="I25" s="34">
+        <v>42.79</v>
+      </c>
+      <c r="J25" s="34">
+        <v>44.44</v>
+      </c>
+      <c r="K25" s="34">
+        <v>78.72</v>
+      </c>
+      <c r="L25" s="34">
+        <v>53.55</v>
+      </c>
+      <c r="M25" s="34">
+        <v>31.95</v>
+      </c>
+      <c r="N25" s="8"/>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A26" s="5">
+        <v>24</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="34">
+        <v>56.35</v>
+      </c>
+      <c r="D26" s="34">
+        <v>84.8</v>
+      </c>
+      <c r="E26" s="34">
+        <v>23.57</v>
+      </c>
+      <c r="F26" s="34">
+        <v>50.06</v>
+      </c>
+      <c r="G26" s="34">
+        <v>68.27</v>
+      </c>
+      <c r="H26" s="34">
+        <v>48.42</v>
+      </c>
+      <c r="I26" s="34">
+        <v>55.15</v>
+      </c>
+      <c r="J26" s="34">
+        <v>54.59</v>
+      </c>
+      <c r="K26" s="34">
+        <v>84.34</v>
+      </c>
+      <c r="L26" s="34">
+        <v>62.23</v>
+      </c>
+      <c r="M26" s="34">
+        <v>41.29</v>
+      </c>
+      <c r="N26" s="8"/>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A27" s="5">
+        <v>25</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="34">
+        <v>65.94</v>
+      </c>
+      <c r="D27" s="34">
+        <v>92</v>
+      </c>
+      <c r="E27" s="34">
+        <v>29.55</v>
+      </c>
+      <c r="F27" s="34">
+        <v>56.56</v>
+      </c>
+      <c r="G27" s="34">
+        <v>76.930000000000007</v>
+      </c>
+      <c r="H27" s="34">
+        <v>60.82</v>
+      </c>
+      <c r="I27" s="34">
+        <v>63.82</v>
+      </c>
+      <c r="J27" s="34">
+        <v>62.17</v>
+      </c>
+      <c r="K27" s="34">
+        <v>87.78</v>
+      </c>
+      <c r="L27" s="34">
+        <v>69.64</v>
+      </c>
+      <c r="M27" s="34">
+        <v>49.55</v>
+      </c>
+      <c r="N27" s="8"/>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A28" s="5">
+        <v>26</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="34">
+        <v>76.42</v>
+      </c>
+      <c r="D28" s="34">
+        <v>94.95</v>
+      </c>
+      <c r="E28" s="34">
+        <v>36.39</v>
+      </c>
+      <c r="F28" s="34">
+        <v>63.97</v>
+      </c>
+      <c r="G28" s="34">
+        <v>82.76</v>
+      </c>
+      <c r="H28" s="34">
+        <v>70.08</v>
+      </c>
+      <c r="I28" s="34">
+        <v>70.17</v>
+      </c>
+      <c r="J28" s="34">
+        <v>67.150000000000006</v>
+      </c>
+      <c r="K28" s="34">
+        <v>90.63</v>
+      </c>
+      <c r="L28" s="34">
+        <v>73.72</v>
+      </c>
+      <c r="M28" s="34">
         <v>55.87</v>
       </c>
       <c r="N28" s="8"/>

</xml_diff>

<commit_message>
add all curve in avearage
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/科研/Research/Code/COOP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/科研/ICCV 23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD5449A-9BA9-3145-9914-30F52422FA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD611D02-9B1D-A844-8E33-D259156A060D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="imcls_fewshot" sheetId="1" r:id="rId1"/>
@@ -60,6 +60,184 @@
       </text>
     </comment>
     <comment ref="M28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>======
+ID#AAAASc0lCiw
+    (2021-12-06 01:16:10)
+lambda around 0.001</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{8E7911B3-3CD9-C347-8EBD-71106A54D73B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">======
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ID#AAAASc0lCi4
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Implementation Details    (2021-12-06 01:16:10)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1. Extract ResNet50 CLIP features (visual encoder with dim=1024)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">2. 1/2/4/8/16-shot training corresponds to 1/2/4/4/4-shot for validation set.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">3. Since no validation set for ImageNet, we make use of hyperparam of Caltech-101 for ImageNet.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>4. Every experiment runs 3 seeds to compute mean/std.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M33" authorId="0" shapeId="0" xr:uid="{E3BEAF1C-A875-B147-BC9F-9815BCD45AEB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>======
+ID#AAAASc0lCiw
+    (2021-12-06 01:16:10)
+lambda around 0.001</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B34" authorId="0" shapeId="0" xr:uid="{C97F81B1-370E-AC47-B00A-3BE4626945D9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">======
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ID#AAAASc0lCi4
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Implementation Details    (2021-12-06 01:16:10)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1. Extract ResNet50 CLIP features (visual encoder with dim=1024)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">2. 1/2/4/8/16-shot training corresponds to 1/2/4/4/4-shot for validation set.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">3. Since no validation set for ImageNet, we make use of hyperparam of Caltech-101 for ImageNet.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>4. Every experiment runs 3 seeds to compute mean/std.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M38" authorId="0" shapeId="0" xr:uid="{4F196603-863C-0C4B-9AC8-8815E1EAC449}">
       <text>
         <r>
           <rPr>
@@ -130,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="58">
   <si>
     <t>Index</t>
   </si>
@@ -286,12 +464,56 @@
     <t>Tip-Adapter, shots=16</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Prompt-Adapter-F, shots=1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prompt-Adapter-F, shots=2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prompt-Adapter-F, shots=4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prompt-Adapter-F, shots=8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prompt-Adapter-F, shots=16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tip-Adapter, shots=1</t>
+  </si>
+  <si>
+    <t>Tip-Adapter, shots=4</t>
+  </si>
+  <si>
+    <t>Tip-Adapter, shots=8</t>
+  </si>
+  <si>
+    <t>Tip-Adapter, shots=16</t>
+  </si>
+  <si>
+    <t>Prompt-Adapter, shots=1</t>
+  </si>
+  <si>
+    <t>Prompt-Adapter, shots=4</t>
+  </si>
+  <si>
+    <t>Prompt-Adapter, shots=8</t>
+  </si>
+  <si>
+    <t>Prompt-Adapter, shots=16</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -341,8 +563,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -385,6 +618,18 @@
         <bgColor rgb="FFEAD1DC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -413,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -434,25 +679,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="6" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -482,6 +712,39 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -703,17 +966,18 @@
   </sheetPr>
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E48" sqref="E48"/>
+      <selection pane="topRight" activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="7.33203125" style="4" customWidth="1"/>
     <col min="2" max="2" width="40.5" style="4" customWidth="1"/>
-    <col min="3" max="6" width="14.5" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="14.5" style="4"/>
+    <col min="3" max="6" width="14.5" style="34" customWidth="1"/>
+    <col min="7" max="13" width="14.5" style="34"/>
+    <col min="14" max="16384" width="14.5" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1">
@@ -723,37 +987,37 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="31" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
@@ -767,38 +1031,38 @@
       <c r="B2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="7">
-        <v>85.77</v>
-      </c>
-      <c r="D2" s="7">
-        <v>66.14</v>
-      </c>
-      <c r="E2" s="7">
-        <v>17.28</v>
-      </c>
-      <c r="F2" s="7">
-        <v>42.32</v>
-      </c>
-      <c r="G2" s="7">
-        <v>37.56</v>
-      </c>
-      <c r="H2" s="7">
-        <v>55.61</v>
-      </c>
-      <c r="I2" s="7">
-        <v>77.31</v>
-      </c>
-      <c r="J2" s="7">
-        <v>58.52</v>
-      </c>
-      <c r="K2" s="7">
-        <v>86.29</v>
-      </c>
-      <c r="L2" s="7">
-        <v>61.46</v>
-      </c>
-      <c r="M2" s="7">
-        <v>58.18</v>
+      <c r="C2" s="30">
+        <v>89.13</v>
+      </c>
+      <c r="D2" s="30">
+        <v>70.650000000000006</v>
+      </c>
+      <c r="E2" s="30">
+        <v>24.87</v>
+      </c>
+      <c r="F2" s="30">
+        <v>44.03</v>
+      </c>
+      <c r="G2" s="30">
+        <v>48.26</v>
+      </c>
+      <c r="H2" s="30">
+        <v>65.55</v>
+      </c>
+      <c r="I2" s="30">
+        <v>85.88</v>
+      </c>
+      <c r="J2" s="30">
+        <v>62.58</v>
+      </c>
+      <c r="K2" s="30">
+        <v>93.27</v>
+      </c>
+      <c r="L2" s="30">
+        <v>67.7</v>
+      </c>
+      <c r="M2" s="30">
+        <v>68.790000000000006</v>
       </c>
       <c r="N2" s="8"/>
     </row>
@@ -807,17 +1071,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
       <c r="N3" s="8"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1">
@@ -827,38 +1091,38 @@
       <c r="B4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="10">
-        <v>85.89</v>
-      </c>
-      <c r="D4" s="10">
-        <v>68.12</v>
-      </c>
-      <c r="E4" s="10">
-        <v>9.64</v>
-      </c>
-      <c r="F4" s="10">
-        <v>44.39</v>
-      </c>
-      <c r="G4" s="10">
-        <v>50.63</v>
-      </c>
-      <c r="H4" s="10">
-        <v>55.59</v>
-      </c>
-      <c r="I4" s="10">
-        <v>74.319999999999993</v>
-      </c>
-      <c r="J4" s="10">
-        <v>60.29</v>
-      </c>
-      <c r="K4" s="10">
-        <v>87.53</v>
-      </c>
-      <c r="L4" s="10">
-        <v>61.92</v>
-      </c>
-      <c r="M4" s="10">
-        <v>57.15</v>
+      <c r="C4" s="9">
+        <v>81.099999999999994</v>
+      </c>
+      <c r="D4" s="9">
+        <v>81.75</v>
+      </c>
+      <c r="E4" s="9">
+        <v>25.4</v>
+      </c>
+      <c r="F4" s="9">
+        <v>44.4</v>
+      </c>
+      <c r="G4" s="9">
+        <v>52.5</v>
+      </c>
+      <c r="H4" s="9">
+        <v>66.2</v>
+      </c>
+      <c r="I4" s="9">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="J4" s="9">
+        <v>60.1</v>
+      </c>
+      <c r="K4" s="9">
+        <v>89.2</v>
+      </c>
+      <c r="L4" s="9">
+        <v>67.8</v>
+      </c>
+      <c r="M4" s="9">
+        <v>69.599999999999994</v>
       </c>
       <c r="N4" s="8"/>
     </row>
@@ -869,38 +1133,38 @@
       <c r="B5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="10">
-        <v>82.64</v>
-      </c>
-      <c r="D5" s="10">
-        <v>77.510000000000005</v>
-      </c>
-      <c r="E5" s="10">
-        <v>18.68</v>
-      </c>
-      <c r="F5" s="10">
-        <v>45.15</v>
-      </c>
-      <c r="G5" s="10">
-        <v>61.5</v>
-      </c>
-      <c r="H5" s="10">
-        <v>58.28</v>
-      </c>
-      <c r="I5" s="10">
-        <v>72.489999999999995</v>
-      </c>
-      <c r="J5" s="10">
-        <v>59.48</v>
-      </c>
-      <c r="K5" s="10">
-        <v>87.93</v>
-      </c>
-      <c r="L5" s="10">
-        <v>64.09</v>
-      </c>
-      <c r="M5" s="10">
-        <v>57.81</v>
+      <c r="C5" s="9">
+        <v>84.45</v>
+      </c>
+      <c r="D5" s="9">
+        <v>88.85</v>
+      </c>
+      <c r="E5" s="9">
+        <v>29.1</v>
+      </c>
+      <c r="F5" s="9">
+        <v>52.8</v>
+      </c>
+      <c r="G5" s="9">
+        <v>61.6</v>
+      </c>
+      <c r="H5" s="9">
+        <v>68.900000000000006</v>
+      </c>
+      <c r="I5" s="9">
+        <v>81.7</v>
+      </c>
+      <c r="J5" s="9">
+        <v>65.2</v>
+      </c>
+      <c r="K5" s="9">
+        <v>93.6</v>
+      </c>
+      <c r="L5" s="9">
+        <v>74.3</v>
+      </c>
+      <c r="M5" s="9">
+        <v>69.77</v>
       </c>
       <c r="N5" s="8"/>
     </row>
@@ -911,38 +1175,38 @@
       <c r="B6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="10">
-        <v>86.7</v>
-      </c>
-      <c r="D6" s="10">
-        <v>86.2</v>
-      </c>
-      <c r="E6" s="10">
-        <v>21.87</v>
-      </c>
-      <c r="F6" s="10">
-        <v>53.49</v>
-      </c>
-      <c r="G6" s="10">
-        <v>70.180000000000007</v>
-      </c>
-      <c r="H6" s="10">
-        <v>62.62</v>
-      </c>
-      <c r="I6" s="10">
-        <v>73.33</v>
-      </c>
-      <c r="J6" s="10">
-        <v>63.47</v>
-      </c>
-      <c r="K6" s="10">
-        <v>89.55</v>
-      </c>
-      <c r="L6" s="10">
-        <v>67.03</v>
-      </c>
-      <c r="M6" s="10">
-        <v>59.99</v>
+      <c r="C6" s="9">
+        <v>90.4</v>
+      </c>
+      <c r="D6" s="9">
+        <v>91.1</v>
+      </c>
+      <c r="E6" s="9">
+        <v>33.9</v>
+      </c>
+      <c r="F6" s="9">
+        <v>58.7</v>
+      </c>
+      <c r="G6" s="9">
+        <v>72</v>
+      </c>
+      <c r="H6" s="9">
+        <v>73.5</v>
+      </c>
+      <c r="I6" s="9">
+        <v>82.4</v>
+      </c>
+      <c r="J6" s="9">
+        <v>69.5</v>
+      </c>
+      <c r="K6" s="9">
+        <v>94</v>
+      </c>
+      <c r="L6" s="9">
+        <v>77.3</v>
+      </c>
+      <c r="M6" s="9">
+        <v>70.37</v>
       </c>
       <c r="N6" s="8"/>
     </row>
@@ -953,38 +1217,36 @@
       <c r="B7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="10">
-        <v>85.32</v>
-      </c>
-      <c r="D7" s="10">
-        <v>91.18</v>
-      </c>
-      <c r="E7" s="10">
-        <v>26.13</v>
-      </c>
-      <c r="F7" s="10">
-        <v>59.97</v>
-      </c>
-      <c r="G7" s="10">
-        <v>76.73</v>
-      </c>
-      <c r="H7" s="10">
-        <v>68.430000000000007</v>
-      </c>
-      <c r="I7" s="10">
-        <v>71.819999999999993</v>
-      </c>
-      <c r="J7" s="10">
-        <v>65.52</v>
-      </c>
-      <c r="K7" s="10">
-        <v>90.21</v>
-      </c>
-      <c r="L7" s="10">
-        <v>71.94</v>
-      </c>
-      <c r="M7" s="10">
-        <v>61.56</v>
+      <c r="C7" s="9">
+        <v>91.65</v>
+      </c>
+      <c r="D7" s="9">
+        <v>93.15</v>
+      </c>
+      <c r="E7" s="9">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="F7" s="9">
+        <v>62.6</v>
+      </c>
+      <c r="G7" s="9">
+        <v>75.900000000000006</v>
+      </c>
+      <c r="H7" s="9">
+        <v>76.3</v>
+      </c>
+      <c r="I7" s="9">
+        <v>83.3</v>
+      </c>
+      <c r="J7" s="9">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="K7" s="9">
+        <v>94.5</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9">
+        <v>70.83</v>
       </c>
       <c r="N7" s="8"/>
     </row>
@@ -995,38 +1257,38 @@
       <c r="B8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="10">
-        <v>87.01</v>
-      </c>
-      <c r="D8" s="10">
-        <v>94.51</v>
-      </c>
-      <c r="E8" s="10">
-        <v>31.26</v>
-      </c>
-      <c r="F8" s="10">
-        <v>63.58</v>
-      </c>
-      <c r="G8" s="10">
-        <v>83.53</v>
-      </c>
-      <c r="H8" s="10">
-        <v>73.36</v>
-      </c>
-      <c r="I8" s="10">
-        <v>74.67</v>
-      </c>
-      <c r="J8" s="10">
-        <v>69.260000000000005</v>
-      </c>
-      <c r="K8" s="10">
-        <v>91.83</v>
-      </c>
-      <c r="L8" s="10">
-        <v>75.709999999999994</v>
-      </c>
-      <c r="M8" s="10">
-        <v>62.95</v>
+      <c r="C8" s="9">
+        <v>91.53</v>
+      </c>
+      <c r="D8" s="9">
+        <v>96.4</v>
+      </c>
+      <c r="E8" s="9">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="F8" s="9">
+        <v>69.47</v>
+      </c>
+      <c r="G8" s="9">
+        <v>84</v>
+      </c>
+      <c r="H8" s="9">
+        <v>79.2</v>
+      </c>
+      <c r="I8" s="9">
+        <v>85</v>
+      </c>
+      <c r="J8" s="9">
+        <v>74.430000000000007</v>
+      </c>
+      <c r="K8" s="9">
+        <v>95.7</v>
+      </c>
+      <c r="L8" s="9">
+        <v>82.4</v>
+      </c>
+      <c r="M8" s="9">
+        <v>71.599999999999994</v>
       </c>
       <c r="N8" s="8"/>
     </row>
@@ -1034,41 +1296,41 @@
       <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="12">
-        <v>85.55</v>
-      </c>
-      <c r="D9" s="12">
-        <v>69.48</v>
-      </c>
-      <c r="E9" s="12">
-        <v>6.58</v>
-      </c>
-      <c r="F9" s="12">
-        <v>41.86</v>
-      </c>
-      <c r="G9" s="12">
-        <v>53.26</v>
-      </c>
-      <c r="H9" s="12">
-        <v>56.02</v>
-      </c>
-      <c r="I9" s="12">
-        <v>72.430000000000007</v>
-      </c>
-      <c r="J9" s="12">
-        <v>59.28</v>
-      </c>
-      <c r="K9" s="12">
-        <v>86.52</v>
-      </c>
-      <c r="L9" s="12">
-        <v>61.47</v>
-      </c>
-      <c r="M9" s="12">
-        <v>57.33</v>
+      <c r="C9" s="10">
+        <v>89.37</v>
+      </c>
+      <c r="D9" s="10">
+        <v>76.08</v>
+      </c>
+      <c r="E9" s="10">
+        <v>27.36</v>
+      </c>
+      <c r="F9" s="10">
+        <v>50.94</v>
+      </c>
+      <c r="G9" s="10">
+        <v>65.09</v>
+      </c>
+      <c r="H9" s="10">
+        <v>67.14</v>
+      </c>
+      <c r="I9" s="10">
+        <v>85.29</v>
+      </c>
+      <c r="J9" s="10">
+        <v>69.040000000000006</v>
+      </c>
+      <c r="K9" s="10">
+        <v>94.19</v>
+      </c>
+      <c r="L9" s="10">
+        <v>72.98</v>
+      </c>
+      <c r="M9" s="10">
+        <v>69.91</v>
       </c>
       <c r="N9" s="8"/>
     </row>
@@ -1076,41 +1338,41 @@
       <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="12">
-        <v>80.569999999999993</v>
-      </c>
-      <c r="D10" s="12">
-        <v>79.400000000000006</v>
-      </c>
-      <c r="E10" s="12">
-        <v>14.18</v>
-      </c>
-      <c r="F10" s="12">
-        <v>45.92</v>
-      </c>
-      <c r="G10" s="12">
-        <v>60.68</v>
-      </c>
-      <c r="H10" s="12">
-        <v>57.09</v>
-      </c>
-      <c r="I10" s="12">
-        <v>71.06</v>
-      </c>
-      <c r="J10" s="12">
-        <v>59.55</v>
-      </c>
-      <c r="K10" s="12">
-        <v>87.3</v>
-      </c>
-      <c r="L10" s="12">
-        <v>65.05</v>
-      </c>
-      <c r="M10" s="12">
-        <v>58.42</v>
+      <c r="C10" s="10">
+        <v>90.7</v>
+      </c>
+      <c r="D10" s="10">
+        <v>83.92</v>
+      </c>
+      <c r="E10" s="10">
+        <v>30.12</v>
+      </c>
+      <c r="F10" s="10">
+        <v>52.01</v>
+      </c>
+      <c r="G10" s="10">
+        <v>75.81</v>
+      </c>
+      <c r="H10" s="10">
+        <v>68.36</v>
+      </c>
+      <c r="I10" s="10">
+        <v>86.32</v>
+      </c>
+      <c r="J10" s="10">
+        <v>69.44</v>
+      </c>
+      <c r="K10" s="10">
+        <v>94.03</v>
+      </c>
+      <c r="L10" s="10">
+        <v>74.91</v>
+      </c>
+      <c r="M10" s="10">
+        <v>70.28</v>
       </c>
       <c r="N10" s="8"/>
     </row>
@@ -1118,41 +1380,41 @@
       <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="12">
-        <v>86.06</v>
-      </c>
-      <c r="D11" s="12">
-        <v>86.52</v>
-      </c>
-      <c r="E11" s="12">
-        <v>22.02</v>
-      </c>
-      <c r="F11" s="12">
-        <v>52.72</v>
-      </c>
-      <c r="G11" s="12">
-        <v>70.930000000000007</v>
-      </c>
-      <c r="H11" s="12">
-        <v>61.62</v>
-      </c>
-      <c r="I11" s="12">
-        <v>72.64</v>
-      </c>
-      <c r="J11" s="12">
-        <v>63.67</v>
-      </c>
-      <c r="K11" s="12">
-        <v>88.53</v>
-      </c>
-      <c r="L11" s="12">
-        <v>67.06</v>
-      </c>
-      <c r="M11" s="12">
-        <v>59.96</v>
+      <c r="C11" s="10">
+        <v>92.75</v>
+      </c>
+      <c r="D11" s="10">
+        <v>90.37</v>
+      </c>
+      <c r="E11" s="10">
+        <v>32.46</v>
+      </c>
+      <c r="F11" s="10">
+        <v>59.21</v>
+      </c>
+      <c r="G11" s="10">
+        <v>82.82</v>
+      </c>
+      <c r="H11" s="10">
+        <v>68.84</v>
+      </c>
+      <c r="I11" s="10">
+        <v>87.04</v>
+      </c>
+      <c r="J11" s="10">
+        <v>70.87</v>
+      </c>
+      <c r="K11" s="10">
+        <v>94.76</v>
+      </c>
+      <c r="L11" s="10">
+        <v>76.97</v>
+      </c>
+      <c r="M11" s="10">
+        <v>70.510000000000005</v>
       </c>
       <c r="N11" s="8"/>
     </row>
@@ -1160,41 +1422,41 @@
       <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="12">
-        <v>83.58</v>
-      </c>
-      <c r="D12" s="12">
-        <v>91.81</v>
-      </c>
-      <c r="E12" s="12">
-        <v>28.18</v>
-      </c>
-      <c r="F12" s="12">
-        <v>59.14</v>
-      </c>
-      <c r="G12" s="12">
-        <v>77.650000000000006</v>
-      </c>
-      <c r="H12" s="12">
-        <v>67.319999999999993</v>
-      </c>
-      <c r="I12" s="12">
-        <v>72.040000000000006</v>
-      </c>
-      <c r="J12" s="12">
-        <v>65.64</v>
-      </c>
-      <c r="K12" s="12">
-        <v>90.33</v>
-      </c>
-      <c r="L12" s="12">
-        <v>72.739999999999995</v>
-      </c>
-      <c r="M12" s="12">
-        <v>62.04</v>
+      <c r="C12" s="10">
+        <v>92.36</v>
+      </c>
+      <c r="D12" s="10">
+        <v>93.91</v>
+      </c>
+      <c r="E12" s="10">
+        <v>37.409999999999997</v>
+      </c>
+      <c r="F12" s="10">
+        <v>63.41</v>
+      </c>
+      <c r="G12" s="10">
+        <v>87.07</v>
+      </c>
+      <c r="H12" s="10">
+        <v>74.69</v>
+      </c>
+      <c r="I12" s="10">
+        <v>87.02</v>
+      </c>
+      <c r="J12" s="10">
+        <v>72.52</v>
+      </c>
+      <c r="K12" s="10">
+        <v>95.05</v>
+      </c>
+      <c r="L12" s="10">
+        <v>80.28</v>
+      </c>
+      <c r="M12" s="10">
+        <v>70.930000000000007</v>
       </c>
       <c r="N12" s="8"/>
     </row>
@@ -1202,41 +1464,41 @@
       <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="12">
-        <v>86.16</v>
-      </c>
-      <c r="D13" s="12">
-        <v>94.8</v>
-      </c>
-      <c r="E13" s="12">
-        <v>32.29</v>
-      </c>
-      <c r="F13" s="12">
-        <v>63.16</v>
-      </c>
-      <c r="G13" s="12">
-        <v>83.55</v>
-      </c>
-      <c r="H13" s="12">
-        <v>73.27</v>
-      </c>
-      <c r="I13" s="12">
-        <v>74.459999999999994</v>
-      </c>
-      <c r="J13" s="12">
-        <v>69.12</v>
-      </c>
-      <c r="K13" s="12">
-        <v>91.62</v>
-      </c>
-      <c r="L13" s="12">
-        <v>75.290000000000006</v>
-      </c>
-      <c r="M13" s="12">
-        <v>63.08</v>
+      <c r="C13" s="10">
+        <v>92.95</v>
+      </c>
+      <c r="D13" s="10">
+        <v>97.11</v>
+      </c>
+      <c r="E13" s="10">
+        <v>46.8</v>
+      </c>
+      <c r="F13" s="10">
+        <v>70.650000000000006</v>
+      </c>
+      <c r="G13" s="10">
+        <v>90.51</v>
+      </c>
+      <c r="H13" s="10">
+        <v>84.33</v>
+      </c>
+      <c r="I13" s="10">
+        <v>85</v>
+      </c>
+      <c r="J13" s="10">
+        <v>75.92</v>
+      </c>
+      <c r="K13" s="10">
+        <v>95.94</v>
+      </c>
+      <c r="L13" s="10">
+        <v>84.03</v>
+      </c>
+      <c r="M13" s="10">
+        <v>72.63</v>
       </c>
       <c r="N13" s="8"/>
     </row>
@@ -1244,41 +1506,41 @@
       <c r="A14" s="5">
         <v>12</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="14">
-        <v>64.650000000000006</v>
-      </c>
-      <c r="D14" s="14">
-        <v>62.89</v>
-      </c>
-      <c r="E14" s="14">
-        <v>14.61</v>
-      </c>
-      <c r="F14" s="14">
-        <v>31.54</v>
-      </c>
-      <c r="G14" s="14">
-        <v>49.67</v>
-      </c>
-      <c r="H14" s="14">
-        <v>34.14</v>
-      </c>
-      <c r="I14" s="14">
-        <v>50.63</v>
-      </c>
-      <c r="J14" s="14">
-        <v>36.950000000000003</v>
-      </c>
-      <c r="K14" s="14">
-        <v>71.400000000000006</v>
-      </c>
-      <c r="L14" s="14">
-        <v>45.04</v>
-      </c>
-      <c r="M14" s="14">
-        <v>32.4</v>
+      <c r="C14" s="11">
+        <v>91.25</v>
+      </c>
+      <c r="D14" s="11">
+        <v>86.89</v>
+      </c>
+      <c r="E14" s="11">
+        <v>30.12</v>
+      </c>
+      <c r="F14" s="11">
+        <v>52.9</v>
+      </c>
+      <c r="G14" s="11">
+        <v>64.98</v>
+      </c>
+      <c r="H14" s="11">
+        <v>68.040000000000006</v>
+      </c>
+      <c r="I14" s="11">
+        <v>86.09</v>
+      </c>
+      <c r="J14" s="11">
+        <v>67.13</v>
+      </c>
+      <c r="K14" s="11">
+        <v>93.79</v>
+      </c>
+      <c r="L14" s="11">
+        <v>73.650000000000006</v>
+      </c>
+      <c r="M14" s="11">
+        <v>69.819999999999993</v>
       </c>
       <c r="N14" s="8"/>
     </row>
@@ -1286,41 +1548,41 @@
       <c r="A15" s="5">
         <v>13</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="14">
-        <v>66.89</v>
-      </c>
-      <c r="D15" s="14">
-        <v>78.819999999999993</v>
-      </c>
-      <c r="E15" s="14">
-        <v>17.7</v>
-      </c>
-      <c r="F15" s="14">
-        <v>39.64</v>
-      </c>
-      <c r="G15" s="14">
-        <v>58.45</v>
-      </c>
-      <c r="H15" s="14">
-        <v>42.39</v>
-      </c>
-      <c r="I15" s="14">
-        <v>54.86</v>
-      </c>
-      <c r="J15" s="14">
-        <v>45.19</v>
-      </c>
-      <c r="K15" s="14">
-        <v>76.56</v>
-      </c>
-      <c r="L15" s="14">
-        <v>52.96</v>
-      </c>
-      <c r="M15" s="14">
-        <v>38.799999999999997</v>
+      <c r="C15" s="11">
+        <v>91.69</v>
+      </c>
+      <c r="D15" s="11">
+        <v>90.01</v>
+      </c>
+      <c r="E15" s="11">
+        <v>33.24</v>
+      </c>
+      <c r="F15" s="11">
+        <v>55.5</v>
+      </c>
+      <c r="G15" s="11">
+        <v>72</v>
+      </c>
+      <c r="H15" s="11">
+        <v>70.95</v>
+      </c>
+      <c r="I15" s="11">
+        <v>86.29</v>
+      </c>
+      <c r="J15" s="11">
+        <v>68.69</v>
+      </c>
+      <c r="K15" s="11">
+        <v>94.44</v>
+      </c>
+      <c r="L15" s="11">
+        <v>76.08</v>
+      </c>
+      <c r="M15" s="11">
+        <v>69.98</v>
       </c>
       <c r="N15" s="8"/>
     </row>
@@ -1328,41 +1590,41 @@
       <c r="A16" s="5">
         <v>14</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="14">
-        <v>74.91</v>
-      </c>
-      <c r="D16" s="14">
-        <v>87.1</v>
-      </c>
-      <c r="E16" s="14">
-        <v>22.9</v>
-      </c>
-      <c r="F16" s="14">
-        <v>49.96</v>
-      </c>
-      <c r="G16" s="14">
-        <v>70.45</v>
-      </c>
-      <c r="H16" s="14">
-        <v>53.33</v>
-      </c>
-      <c r="I16" s="14">
-        <v>60.26</v>
-      </c>
-      <c r="J16" s="14">
-        <v>53.31</v>
-      </c>
-      <c r="K16" s="14">
-        <v>83.42</v>
-      </c>
-      <c r="L16" s="14">
-        <v>60.36</v>
-      </c>
-      <c r="M16" s="14">
-        <v>44.93</v>
+      <c r="C16" s="11">
+        <v>92.23</v>
+      </c>
+      <c r="D16" s="11">
+        <v>92.98</v>
+      </c>
+      <c r="E16" s="11">
+        <v>35.67</v>
+      </c>
+      <c r="F16" s="11">
+        <v>61.76</v>
+      </c>
+      <c r="G16" s="11">
+        <v>78.63</v>
+      </c>
+      <c r="H16" s="11">
+        <v>74.36</v>
+      </c>
+      <c r="I16" s="11">
+        <v>86.7</v>
+      </c>
+      <c r="J16" s="11">
+        <v>70.66</v>
+      </c>
+      <c r="K16" s="11">
+        <v>94.93</v>
+      </c>
+      <c r="L16" s="11">
+        <v>79.8</v>
+      </c>
+      <c r="M16" s="11">
+        <v>70.11</v>
       </c>
       <c r="N16" s="8"/>
     </row>
@@ -1370,41 +1632,41 @@
       <c r="A17" s="5">
         <v>15</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="14">
-        <v>76.12</v>
-      </c>
-      <c r="D17" s="14">
-        <v>92.61</v>
-      </c>
-      <c r="E17" s="14">
-        <v>29.52</v>
-      </c>
-      <c r="F17" s="14">
-        <v>58.33</v>
-      </c>
-      <c r="G17" s="14">
-        <v>78</v>
-      </c>
-      <c r="H17" s="14">
-        <v>63.06</v>
-      </c>
-      <c r="I17" s="14">
-        <v>64.52</v>
-      </c>
-      <c r="J17" s="14">
-        <v>58.41</v>
-      </c>
-      <c r="K17" s="14">
-        <v>86.71</v>
-      </c>
-      <c r="L17" s="14">
-        <v>67.42</v>
-      </c>
-      <c r="M17" s="14">
-        <v>50.11</v>
+      <c r="C17" s="11">
+        <v>92.48</v>
+      </c>
+      <c r="D17" s="11">
+        <v>95.62</v>
+      </c>
+      <c r="E17" s="11">
+        <v>40.98</v>
+      </c>
+      <c r="F17" s="11">
+        <v>67.319999999999993</v>
+      </c>
+      <c r="G17" s="11">
+        <v>82.25</v>
+      </c>
+      <c r="H17" s="11">
+        <v>77.760000000000005</v>
+      </c>
+      <c r="I17" s="11">
+        <v>86.91</v>
+      </c>
+      <c r="J17" s="11">
+        <v>73.89</v>
+      </c>
+      <c r="K17" s="11">
+        <v>95.21</v>
+      </c>
+      <c r="L17" s="11">
+        <v>82.63</v>
+      </c>
+      <c r="M17" s="11">
+        <v>71.72</v>
       </c>
       <c r="N17" s="8"/>
     </row>
@@ -1412,41 +1674,41 @@
       <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="14">
-        <v>81.099999999999994</v>
-      </c>
-      <c r="D18" s="14">
-        <v>95.59</v>
-      </c>
-      <c r="E18" s="14">
-        <v>36.93</v>
-      </c>
-      <c r="F18" s="14">
-        <v>62.87</v>
-      </c>
-      <c r="G18" s="14">
-        <v>84.55</v>
-      </c>
-      <c r="H18" s="14">
-        <v>72.2</v>
-      </c>
-      <c r="I18" s="14">
-        <v>70.02</v>
-      </c>
-      <c r="J18" s="14">
-        <v>63.83</v>
-      </c>
-      <c r="K18" s="14">
-        <v>90.58</v>
-      </c>
-      <c r="L18" s="14">
-        <v>73.23</v>
-      </c>
-      <c r="M18" s="14">
-        <v>54.57</v>
+      <c r="C18" s="11">
+        <v>93.08</v>
+      </c>
+      <c r="D18" s="11">
+        <v>96.31</v>
+      </c>
+      <c r="E18" s="11">
+        <v>45.45</v>
+      </c>
+      <c r="F18" s="11">
+        <v>71.930000000000007</v>
+      </c>
+      <c r="G18" s="11">
+        <v>87.43</v>
+      </c>
+      <c r="H18" s="11">
+        <v>83.82</v>
+      </c>
+      <c r="I18" s="11">
+        <v>87.38</v>
+      </c>
+      <c r="J18" s="11">
+        <v>76.3</v>
+      </c>
+      <c r="K18" s="11">
+        <v>95.94</v>
+      </c>
+      <c r="L18" s="11">
+        <v>85.01</v>
+      </c>
+      <c r="M18" s="11">
+        <v>73.45</v>
       </c>
       <c r="N18" s="8"/>
     </row>
@@ -1454,41 +1716,41 @@
       <c r="A19" s="5">
         <v>17</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="16">
-        <v>65.069999999999993</v>
-      </c>
-      <c r="D19" s="16">
-        <v>62.58</v>
-      </c>
-      <c r="E19" s="16">
-        <v>14.04</v>
-      </c>
-      <c r="F19" s="16">
-        <v>28.92</v>
-      </c>
-      <c r="G19" s="16">
-        <v>48.79</v>
-      </c>
-      <c r="H19" s="16">
-        <v>34.26</v>
-      </c>
-      <c r="I19" s="16">
-        <v>46.92</v>
-      </c>
-      <c r="J19" s="16">
-        <v>35.659999999999997</v>
-      </c>
-      <c r="K19" s="16">
-        <v>69.2</v>
-      </c>
-      <c r="L19" s="16">
-        <v>42.72</v>
-      </c>
-      <c r="M19" s="16">
-        <v>31.01</v>
+      <c r="B19" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="12">
+        <v>87.84</v>
+      </c>
+      <c r="D19" s="12">
+        <v>95.9</v>
+      </c>
+      <c r="E19" s="12">
+        <v>43.2</v>
+      </c>
+      <c r="F19" s="12">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="G19" s="12">
+        <v>82.02</v>
+      </c>
+      <c r="H19" s="12">
+        <v>78.489999999999995</v>
+      </c>
+      <c r="I19" s="12">
+        <v>79.540000000000006</v>
+      </c>
+      <c r="J19" s="12">
+        <v>70.91</v>
+      </c>
+      <c r="K19" s="12">
+        <v>93.83</v>
+      </c>
+      <c r="L19" s="12">
+        <v>79.73</v>
+      </c>
+      <c r="M19" s="12">
+        <v>62.42</v>
       </c>
       <c r="N19" s="8"/>
     </row>
@@ -1496,41 +1758,41 @@
       <c r="A20" s="5">
         <v>18</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="16">
-        <v>66.69</v>
-      </c>
-      <c r="D20" s="16">
-        <v>76.790000000000006</v>
-      </c>
-      <c r="E20" s="16">
-        <v>18.48</v>
-      </c>
-      <c r="F20" s="16">
-        <v>39.659999999999997</v>
-      </c>
-      <c r="G20" s="16">
-        <v>58.99</v>
-      </c>
-      <c r="H20" s="16">
-        <v>42.61</v>
-      </c>
-      <c r="I20" s="16">
-        <v>53.06</v>
-      </c>
-      <c r="J20" s="16">
-        <v>44.77</v>
-      </c>
-      <c r="K20" s="16">
-        <v>76.650000000000006</v>
-      </c>
-      <c r="L20" s="16">
-        <v>52.28</v>
-      </c>
-      <c r="M20" s="16">
-        <v>38.19</v>
+      <c r="B20" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="12">
+        <v>90.76</v>
+      </c>
+      <c r="D20" s="12">
+        <v>96.71</v>
+      </c>
+      <c r="E20" s="12">
+        <v>43.38</v>
+      </c>
+      <c r="F20" s="12">
+        <v>67.2</v>
+      </c>
+      <c r="G20" s="12">
+        <v>83.36</v>
+      </c>
+      <c r="H20" s="12">
+        <v>80.08</v>
+      </c>
+      <c r="I20" s="12">
+        <v>82.41</v>
+      </c>
+      <c r="J20" s="12">
+        <v>72.25</v>
+      </c>
+      <c r="K20" s="12">
+        <v>94.4</v>
+      </c>
+      <c r="L20" s="12">
+        <v>79.91</v>
+      </c>
+      <c r="M20" s="12">
+        <v>63.91</v>
       </c>
       <c r="N20" s="8"/>
     </row>
@@ -1538,41 +1800,41 @@
       <c r="A21" s="5">
         <v>19</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="16">
-        <v>74.349999999999994</v>
-      </c>
-      <c r="D21" s="16">
-        <v>87.04</v>
-      </c>
-      <c r="E21" s="16">
-        <v>22.92</v>
-      </c>
-      <c r="F21" s="16">
-        <v>50.37</v>
-      </c>
-      <c r="G21" s="16">
-        <v>70.55</v>
-      </c>
-      <c r="H21" s="16">
-        <v>53.68</v>
-      </c>
-      <c r="I21" s="16">
-        <v>59.71</v>
-      </c>
-      <c r="J21" s="16">
-        <v>53.04</v>
-      </c>
-      <c r="K21" s="16">
-        <v>83.31</v>
-      </c>
-      <c r="L21" s="16">
-        <v>59.23</v>
-      </c>
-      <c r="M21" s="16">
-        <v>44.67</v>
+      <c r="B21" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="12">
+        <v>90.32</v>
+      </c>
+      <c r="D21" s="12">
+        <v>96.51</v>
+      </c>
+      <c r="E21" s="12">
+        <v>43.83</v>
+      </c>
+      <c r="F21" s="12">
+        <v>69.209999999999994</v>
+      </c>
+      <c r="G21" s="12">
+        <v>80.42</v>
+      </c>
+      <c r="H21" s="12">
+        <v>80.33</v>
+      </c>
+      <c r="I21" s="12">
+        <v>83.68</v>
+      </c>
+      <c r="J21" s="12">
+        <v>73.209999999999994</v>
+      </c>
+      <c r="K21" s="12">
+        <v>95.25</v>
+      </c>
+      <c r="L21" s="12">
+        <v>81.650000000000006</v>
+      </c>
+      <c r="M21" s="12">
+        <v>67.790000000000006</v>
       </c>
       <c r="N21" s="8"/>
     </row>
@@ -1580,41 +1842,41 @@
       <c r="A22" s="5">
         <v>20</v>
       </c>
-      <c r="B22" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="16">
-        <v>75.959999999999994</v>
-      </c>
-      <c r="D22" s="16">
-        <v>92.53</v>
-      </c>
-      <c r="E22" s="16">
-        <v>29.47</v>
-      </c>
-      <c r="F22" s="16">
-        <v>57.84</v>
-      </c>
-      <c r="G22" s="16">
-        <v>78.37</v>
-      </c>
-      <c r="H22" s="16">
-        <v>63.22</v>
-      </c>
-      <c r="I22" s="16">
-        <v>64.55</v>
-      </c>
-      <c r="J22" s="16">
-        <v>58.31</v>
-      </c>
-      <c r="K22" s="16">
-        <v>86.33</v>
-      </c>
-      <c r="L22" s="16">
-        <v>67.97</v>
-      </c>
-      <c r="M22" s="16">
-        <v>50.29</v>
+      <c r="B22" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="12">
+        <v>91.31</v>
+      </c>
+      <c r="D22" s="12">
+        <v>97.2</v>
+      </c>
+      <c r="E22" s="12">
+        <v>45.84</v>
+      </c>
+      <c r="F22" s="12">
+        <v>69.209999999999994</v>
+      </c>
+      <c r="G22" s="12">
+        <v>82.68</v>
+      </c>
+      <c r="H22" s="12">
+        <v>81.53</v>
+      </c>
+      <c r="I22" s="12">
+        <v>84.81</v>
+      </c>
+      <c r="J22" s="12">
+        <v>74.11</v>
+      </c>
+      <c r="K22" s="12">
+        <v>95.38</v>
+      </c>
+      <c r="L22" s="12">
+        <v>83</v>
+      </c>
+      <c r="M22" s="12">
+        <v>70.290000000000006</v>
       </c>
       <c r="N22" s="8"/>
     </row>
@@ -1622,41 +1884,41 @@
       <c r="A23" s="5">
         <v>21</v>
       </c>
-      <c r="B23" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="16">
-        <v>80.87</v>
-      </c>
-      <c r="D23" s="16">
-        <v>95.52</v>
-      </c>
-      <c r="E23" s="16">
-        <v>37.479999999999997</v>
-      </c>
-      <c r="F23" s="16">
-        <v>62.57</v>
-      </c>
-      <c r="G23" s="16">
-        <v>84.87</v>
-      </c>
-      <c r="H23" s="16">
-        <v>72.319999999999993</v>
-      </c>
-      <c r="I23" s="16">
-        <v>70.040000000000006</v>
-      </c>
-      <c r="J23" s="16">
-        <v>63.76</v>
-      </c>
-      <c r="K23" s="16">
-        <v>90.57</v>
-      </c>
-      <c r="L23" s="16">
-        <v>73.349999999999994</v>
-      </c>
-      <c r="M23" s="16">
-        <v>54.65</v>
+      <c r="B23" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="12">
+        <v>91.66</v>
+      </c>
+      <c r="D23" s="12">
+        <v>97.89</v>
+      </c>
+      <c r="E23" s="12">
+        <v>48.39</v>
+      </c>
+      <c r="F23" s="12">
+        <v>71.28</v>
+      </c>
+      <c r="G23" s="12">
+        <v>85.37</v>
+      </c>
+      <c r="H23" s="12">
+        <v>82.91</v>
+      </c>
+      <c r="I23" s="12">
+        <v>86.35</v>
+      </c>
+      <c r="J23" s="12">
+        <v>75.56</v>
+      </c>
+      <c r="K23" s="12">
+        <v>95.82</v>
+      </c>
+      <c r="L23" s="12">
+        <v>84.43</v>
+      </c>
+      <c r="M23" s="12">
+        <v>71.88</v>
       </c>
       <c r="N23" s="8"/>
     </row>
@@ -1664,40 +1926,40 @@
       <c r="A24" s="5">
         <v>22</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="33">
         <v>30.14</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="33">
         <v>58.07</v>
       </c>
-      <c r="E24" s="18">
+      <c r="E24" s="33">
         <v>12.89</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="33">
         <v>29.59</v>
       </c>
-      <c r="G24" s="18">
+      <c r="G24" s="33">
         <v>51</v>
       </c>
-      <c r="H24" s="18">
+      <c r="H24" s="33">
         <v>24.64</v>
       </c>
-      <c r="I24" s="18">
+      <c r="I24" s="33">
         <v>30.13</v>
       </c>
-      <c r="J24" s="18">
+      <c r="J24" s="33">
         <v>32.799999999999997</v>
       </c>
-      <c r="K24" s="18">
+      <c r="K24" s="33">
         <v>70.62</v>
       </c>
-      <c r="L24" s="18">
+      <c r="L24" s="33">
         <v>41.43</v>
       </c>
-      <c r="M24" s="18">
+      <c r="M24" s="33">
         <v>22.07</v>
       </c>
       <c r="N24" s="8"/>
@@ -1706,40 +1968,40 @@
       <c r="A25" s="5">
         <v>23</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="18">
+      <c r="C25" s="33">
         <v>43.47</v>
       </c>
-      <c r="D25" s="18">
+      <c r="D25" s="33">
         <v>73.349999999999994</v>
       </c>
-      <c r="E25" s="18">
+      <c r="E25" s="33">
         <v>17.850000000000001</v>
       </c>
-      <c r="F25" s="18">
+      <c r="F25" s="33">
         <v>39.479999999999997</v>
       </c>
-      <c r="G25" s="18">
+      <c r="G25" s="33">
         <v>61.58</v>
       </c>
-      <c r="H25" s="18">
+      <c r="H25" s="33">
         <v>36.53</v>
       </c>
-      <c r="I25" s="18">
+      <c r="I25" s="33">
         <v>42.79</v>
       </c>
-      <c r="J25" s="18">
+      <c r="J25" s="33">
         <v>44.44</v>
       </c>
-      <c r="K25" s="18">
+      <c r="K25" s="33">
         <v>78.72</v>
       </c>
-      <c r="L25" s="18">
+      <c r="L25" s="33">
         <v>53.55</v>
       </c>
-      <c r="M25" s="18">
+      <c r="M25" s="33">
         <v>31.95</v>
       </c>
       <c r="N25" s="8"/>
@@ -1748,40 +2010,40 @@
       <c r="A26" s="5">
         <v>24</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="33">
         <v>56.35</v>
       </c>
-      <c r="D26" s="18">
+      <c r="D26" s="33">
         <v>84.8</v>
       </c>
-      <c r="E26" s="18">
+      <c r="E26" s="33">
         <v>23.57</v>
       </c>
-      <c r="F26" s="18">
+      <c r="F26" s="33">
         <v>50.06</v>
       </c>
-      <c r="G26" s="18">
+      <c r="G26" s="33">
         <v>68.27</v>
       </c>
-      <c r="H26" s="18">
+      <c r="H26" s="33">
         <v>48.42</v>
       </c>
-      <c r="I26" s="18">
+      <c r="I26" s="33">
         <v>55.15</v>
       </c>
-      <c r="J26" s="18">
+      <c r="J26" s="33">
         <v>54.59</v>
       </c>
-      <c r="K26" s="18">
+      <c r="K26" s="33">
         <v>84.34</v>
       </c>
-      <c r="L26" s="18">
+      <c r="L26" s="33">
         <v>62.23</v>
       </c>
-      <c r="M26" s="18">
+      <c r="M26" s="33">
         <v>41.29</v>
       </c>
       <c r="N26" s="8"/>
@@ -1790,40 +2052,40 @@
       <c r="A27" s="5">
         <v>25</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="33">
         <v>65.94</v>
       </c>
-      <c r="D27" s="18">
+      <c r="D27" s="33">
         <v>92</v>
       </c>
-      <c r="E27" s="18">
+      <c r="E27" s="33">
         <v>29.55</v>
       </c>
-      <c r="F27" s="18">
+      <c r="F27" s="33">
         <v>56.56</v>
       </c>
-      <c r="G27" s="18">
+      <c r="G27" s="33">
         <v>76.930000000000007</v>
       </c>
-      <c r="H27" s="18">
+      <c r="H27" s="33">
         <v>60.82</v>
       </c>
-      <c r="I27" s="18">
+      <c r="I27" s="33">
         <v>63.82</v>
       </c>
-      <c r="J27" s="18">
+      <c r="J27" s="33">
         <v>62.17</v>
       </c>
-      <c r="K27" s="18">
+      <c r="K27" s="33">
         <v>87.78</v>
       </c>
-      <c r="L27" s="18">
+      <c r="L27" s="33">
         <v>69.64</v>
       </c>
-      <c r="M27" s="18">
+      <c r="M27" s="33">
         <v>49.55</v>
       </c>
       <c r="N27" s="8"/>
@@ -1832,111 +2094,469 @@
       <c r="A28" s="5">
         <v>26</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="18">
+      <c r="C28" s="33">
         <v>76.42</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D28" s="33">
         <v>94.95</v>
       </c>
-      <c r="E28" s="18">
+      <c r="E28" s="33">
         <v>36.39</v>
       </c>
-      <c r="F28" s="18">
+      <c r="F28" s="33">
         <v>63.97</v>
       </c>
-      <c r="G28" s="18">
+      <c r="G28" s="33">
         <v>82.76</v>
       </c>
-      <c r="H28" s="18">
+      <c r="H28" s="33">
         <v>70.08</v>
       </c>
-      <c r="I28" s="18">
+      <c r="I28" s="33">
         <v>70.17</v>
       </c>
-      <c r="J28" s="18">
+      <c r="J28" s="33">
         <v>67.150000000000006</v>
       </c>
-      <c r="K28" s="18">
+      <c r="K28" s="33">
         <v>90.63</v>
       </c>
-      <c r="L28" s="18">
+      <c r="L28" s="33">
         <v>73.72</v>
       </c>
-      <c r="M28" s="18">
+      <c r="M28" s="33">
         <v>55.87</v>
       </c>
       <c r="N28" s="8"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A29" s="5"/>
+      <c r="A29" s="5">
+        <v>27</v>
+      </c>
+      <c r="B29" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="39">
+        <v>89.29</v>
+      </c>
+      <c r="D29" s="39">
+        <v>83.19</v>
+      </c>
+      <c r="E29" s="39">
+        <v>27.78</v>
+      </c>
+      <c r="F29" s="39">
+        <v>51.18</v>
+      </c>
+      <c r="G29" s="39">
+        <v>64.150000000000006</v>
+      </c>
+      <c r="H29" s="39">
+        <v>66.989999999999995</v>
+      </c>
+      <c r="I29" s="39">
+        <v>85.95</v>
+      </c>
+      <c r="J29" s="39">
+        <v>65.7</v>
+      </c>
+      <c r="K29" s="39">
+        <v>93.43</v>
+      </c>
+      <c r="L29" s="39">
+        <v>69.52</v>
+      </c>
+      <c r="M29" s="39">
+        <v>68.91</v>
+      </c>
       <c r="N29" s="8"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A30" s="5"/>
+      <c r="A30" s="5">
+        <v>28</v>
+      </c>
+      <c r="B30" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="39">
+        <v>89.7</v>
+      </c>
+      <c r="D30" s="39">
+        <v>97.21</v>
+      </c>
+      <c r="E30" s="39">
+        <v>31.56</v>
+      </c>
+      <c r="F30" s="39">
+        <v>52.54</v>
+      </c>
+      <c r="G30" s="39">
+        <v>68.680000000000007</v>
+      </c>
+      <c r="H30" s="39">
+        <v>68.540000000000006</v>
+      </c>
+      <c r="I30" s="39">
+        <v>86.06</v>
+      </c>
+      <c r="J30" s="39">
+        <v>68.040000000000006</v>
+      </c>
+      <c r="K30" s="39">
+        <v>94</v>
+      </c>
+      <c r="L30" s="39">
+        <v>71.05</v>
+      </c>
+      <c r="M30" s="39">
+        <v>69.2</v>
+      </c>
       <c r="N30" s="8"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A31" s="5"/>
+      <c r="A31" s="5">
+        <v>29</v>
+      </c>
+      <c r="B31" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="39">
+        <v>90.98</v>
+      </c>
+      <c r="D31" s="39">
+        <v>91.68</v>
+      </c>
+      <c r="E31" s="39">
+        <v>32.549999999999997</v>
+      </c>
+      <c r="F31" s="39">
+        <v>59.81</v>
+      </c>
+      <c r="G31" s="39">
+        <v>72</v>
+      </c>
+      <c r="H31" s="39">
+        <v>71.11</v>
+      </c>
+      <c r="I31" s="39">
+        <v>86.1</v>
+      </c>
+      <c r="J31" s="39">
+        <v>69.11</v>
+      </c>
+      <c r="K31" s="39">
+        <v>94.81</v>
+      </c>
+      <c r="L31" s="39">
+        <v>74.39</v>
+      </c>
+      <c r="M31" s="39">
+        <v>69.5</v>
+      </c>
       <c r="N31" s="8"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A32" s="5"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
+      <c r="A32" s="5">
+        <v>30</v>
+      </c>
+      <c r="B32" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="39">
+        <v>90.84</v>
+      </c>
+      <c r="D32" s="39">
+        <v>94.07</v>
+      </c>
+      <c r="E32" s="39">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="F32" s="39">
+        <v>63.3</v>
+      </c>
+      <c r="G32" s="39">
+        <v>71.28</v>
+      </c>
+      <c r="H32" s="39">
+        <v>72.25</v>
+      </c>
+      <c r="I32" s="39">
+        <v>86.35</v>
+      </c>
+      <c r="J32" s="39">
+        <v>70.66</v>
+      </c>
+      <c r="K32" s="39">
+        <v>94.44</v>
+      </c>
+      <c r="L32" s="39">
+        <v>76.34</v>
+      </c>
+      <c r="M32" s="39">
+        <v>70.010000000000005</v>
+      </c>
       <c r="N32" s="8"/>
     </row>
     <row r="33" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A33" s="5"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21"/>
+      <c r="A33" s="5">
+        <v>31</v>
+      </c>
+      <c r="B33" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="39">
+        <v>94.57</v>
+      </c>
+      <c r="D33" s="39">
+        <v>94.6</v>
+      </c>
+      <c r="E33" s="39">
+        <v>39.96</v>
+      </c>
+      <c r="F33" s="39">
+        <v>66.08</v>
+      </c>
+      <c r="G33" s="39">
+        <v>78.010000000000005</v>
+      </c>
+      <c r="H33" s="39">
+        <v>75.39</v>
+      </c>
+      <c r="I33" s="39">
+        <v>86.45</v>
+      </c>
+      <c r="J33" s="39">
+        <v>71.94</v>
+      </c>
+      <c r="K33" s="39">
+        <v>95.09</v>
+      </c>
+      <c r="L33" s="39">
+        <v>78.510000000000005</v>
+      </c>
+      <c r="M33" s="39">
+        <v>70.319999999999993</v>
+      </c>
       <c r="N33" s="8"/>
     </row>
     <row r="34" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A34" s="5"/>
-      <c r="N34" s="22"/>
+      <c r="A34" s="5">
+        <v>32</v>
+      </c>
+      <c r="B34" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="41">
+        <v>85.33</v>
+      </c>
+      <c r="D34" s="41">
+        <v>95.9</v>
+      </c>
+      <c r="E34" s="41">
+        <v>39.479999999999997</v>
+      </c>
+      <c r="F34" s="41">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="G34" s="41">
+        <v>80.09</v>
+      </c>
+      <c r="H34" s="41">
+        <v>77.44</v>
+      </c>
+      <c r="I34" s="41">
+        <v>76.8</v>
+      </c>
+      <c r="J34" s="41">
+        <v>69.349999999999994</v>
+      </c>
+      <c r="K34" s="41">
+        <v>93.51</v>
+      </c>
+      <c r="L34" s="41">
+        <v>78.61</v>
+      </c>
+      <c r="M34" s="41">
+        <v>58.76</v>
+      </c>
+      <c r="N34" s="17"/>
     </row>
     <row r="35" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A35" s="5"/>
-      <c r="N35" s="22"/>
+      <c r="A35" s="5">
+        <v>33</v>
+      </c>
+      <c r="B35" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="41">
+        <v>85.46</v>
+      </c>
+      <c r="D35" s="41">
+        <v>94.73</v>
+      </c>
+      <c r="E35" s="41">
+        <v>40.26</v>
+      </c>
+      <c r="F35" s="41">
+        <v>66.48</v>
+      </c>
+      <c r="G35" s="41">
+        <v>80.42</v>
+      </c>
+      <c r="H35" s="41">
+        <v>77.94</v>
+      </c>
+      <c r="I35" s="41">
+        <v>77.17</v>
+      </c>
+      <c r="J35" s="41">
+        <v>69.8</v>
+      </c>
+      <c r="K35" s="41">
+        <v>93.51</v>
+      </c>
+      <c r="L35" s="42">
+        <v>78.72</v>
+      </c>
+      <c r="M35" s="41">
+        <v>58.59</v>
+      </c>
+      <c r="N35" s="17"/>
     </row>
     <row r="36" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A36" s="5"/>
-      <c r="N36" s="22"/>
+      <c r="A36" s="5">
+        <v>34</v>
+      </c>
+      <c r="B36" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="41">
+        <v>85.73</v>
+      </c>
+      <c r="D36" s="41">
+        <v>95.7</v>
+      </c>
+      <c r="E36" s="41">
+        <v>41.22</v>
+      </c>
+      <c r="F36" s="41">
+        <v>68.03</v>
+      </c>
+      <c r="G36" s="41">
+        <v>81.2</v>
+      </c>
+      <c r="H36" s="41">
+        <v>77.55</v>
+      </c>
+      <c r="I36" s="41">
+        <v>77.95</v>
+      </c>
+      <c r="J36" s="41">
+        <v>70.55</v>
+      </c>
+      <c r="K36" s="41">
+        <v>94.08</v>
+      </c>
+      <c r="L36" s="41">
+        <v>78.540000000000006</v>
+      </c>
+      <c r="M36" s="41">
+        <v>58.68</v>
+      </c>
+      <c r="N36" s="17"/>
     </row>
     <row r="37" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A37" s="5"/>
-      <c r="N37" s="22"/>
+      <c r="A37" s="5">
+        <v>35</v>
+      </c>
+      <c r="B37" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="41">
+        <v>85.46</v>
+      </c>
+      <c r="D37" s="41">
+        <v>96.26</v>
+      </c>
+      <c r="E37" s="41">
+        <v>41.4</v>
+      </c>
+      <c r="F37" s="41">
+        <v>68.2</v>
+      </c>
+      <c r="G37" s="41">
+        <v>81.81</v>
+      </c>
+      <c r="H37" s="41">
+        <v>78.349999999999994</v>
+      </c>
+      <c r="I37" s="41">
+        <v>79.489999999999995</v>
+      </c>
+      <c r="J37" s="41">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="K37" s="41">
+        <v>94.28</v>
+      </c>
+      <c r="L37" s="41">
+        <v>79.38</v>
+      </c>
+      <c r="M37" s="41">
+        <v>58.97</v>
+      </c>
+      <c r="N37" s="17"/>
     </row>
     <row r="38" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A38" s="5"/>
-      <c r="N38" s="22"/>
+      <c r="A38" s="5">
+        <v>36</v>
+      </c>
+      <c r="B38" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="41">
+        <v>85.94</v>
+      </c>
+      <c r="D38" s="41">
+        <v>96.43</v>
+      </c>
+      <c r="E38" s="41">
+        <v>43.14</v>
+      </c>
+      <c r="F38" s="41">
+        <v>70.209999999999994</v>
+      </c>
+      <c r="G38" s="41">
+        <v>83.15</v>
+      </c>
+      <c r="H38" s="41">
+        <v>79.59</v>
+      </c>
+      <c r="I38" s="41">
+        <v>81.23</v>
+      </c>
+      <c r="J38" s="41">
+        <v>72.88</v>
+      </c>
+      <c r="K38" s="41">
+        <v>94.52</v>
+      </c>
+      <c r="L38" s="41">
+        <v>80.17</v>
+      </c>
+      <c r="M38" s="41">
+        <v>61.98</v>
+      </c>
+      <c r="N38" s="17"/>
     </row>
     <row r="39" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A39" s="5"/>
-      <c r="N39" s="22"/>
+      <c r="A39" s="5">
+        <v>37</v>
+      </c>
+      <c r="N39" s="17"/>
     </row>
     <row r="40" spans="1:14" ht="15.75" customHeight="1">
       <c r="A40" s="5"/>
@@ -1945,34 +2565,34 @@
     <row r="41" spans="1:14" ht="15.75" customHeight="1">
       <c r="A41" s="5"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24"/>
-      <c r="K41" s="24"/>
-      <c r="L41" s="24"/>
-      <c r="M41" s="24"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="36"/>
+      <c r="J41" s="36"/>
+      <c r="K41" s="36"/>
+      <c r="L41" s="36"/>
+      <c r="M41" s="36"/>
       <c r="N41" s="8"/>
     </row>
     <row r="42" spans="1:14" ht="15.75" customHeight="1">
       <c r="A42" s="5"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
-      <c r="K42" s="21"/>
-      <c r="L42" s="21"/>
-      <c r="M42" s="21"/>
-      <c r="N42" s="22"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="37"/>
+      <c r="L42" s="37"/>
+      <c r="M42" s="37"/>
+      <c r="N42" s="17"/>
     </row>
     <row r="43" spans="1:14" ht="15.75" customHeight="1">
       <c r="N43" s="8"/>
@@ -3346,9 +3966,9 @@
   </sheetPr>
   <dimension ref="A1:N1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F16" sqref="F16"/>
+      <selection pane="topRight" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -3467,120 +4087,120 @@
       <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
       <c r="N4" s="8"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1">
       <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
       <c r="N5" s="8"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1">
       <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
       <c r="N6" s="8"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1">
       <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
       <c r="N7" s="8"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1">
       <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="21">
         <v>87.01</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="21">
         <v>94.51</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="21">
         <v>31.26</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="21">
         <v>63.58</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="21">
         <v>83.53</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H8" s="21">
         <v>73.36</v>
       </c>
-      <c r="I8" s="26">
+      <c r="I8" s="21">
         <v>74.67</v>
       </c>
-      <c r="J8" s="26">
+      <c r="J8" s="21">
         <v>69.260000000000005</v>
       </c>
-      <c r="K8" s="26">
+      <c r="K8" s="21">
         <v>91.83</v>
       </c>
-      <c r="L8" s="26">
+      <c r="L8" s="21">
         <v>75.709999999999994</v>
       </c>
-      <c r="M8" s="26">
+      <c r="M8" s="21">
         <v>62.95</v>
       </c>
       <c r="N8" s="8"/>
@@ -3589,232 +4209,232 @@
       <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
       <c r="N9" s="8"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1">
       <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
       <c r="N10" s="8"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1">
       <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
       <c r="N11" s="8"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1">
       <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
       <c r="N12" s="8"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1">
       <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C13" s="23">
         <v>86.16</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="23">
         <v>94.8</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13" s="23">
         <v>32.29</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="23">
         <v>63.16</v>
       </c>
-      <c r="G13" s="28">
+      <c r="G13" s="23">
         <v>83.55</v>
       </c>
-      <c r="H13" s="28">
+      <c r="H13" s="23">
         <v>73.27</v>
       </c>
-      <c r="I13" s="28">
+      <c r="I13" s="23">
         <v>74.459999999999994</v>
       </c>
-      <c r="J13" s="28">
+      <c r="J13" s="23">
         <v>69.12</v>
       </c>
-      <c r="K13" s="28">
+      <c r="K13" s="23">
         <v>91.62</v>
       </c>
-      <c r="L13" s="28">
+      <c r="L13" s="23">
         <v>75.290000000000006</v>
       </c>
-      <c r="M13" s="28">
+      <c r="M13" s="23">
         <v>63.08</v>
       </c>
       <c r="N13" s="8"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1">
       <c r="A14" s="5"/>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
       <c r="N14" s="8"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1">
       <c r="A15" s="5"/>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
       <c r="N15" s="8"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1">
       <c r="A16" s="5"/>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
       <c r="N16" s="8"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1">
       <c r="A17" s="5"/>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
       <c r="N17" s="8"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1">
       <c r="A18" s="5"/>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="28">
+      <c r="C18" s="23">
         <v>86.16</v>
       </c>
-      <c r="D18" s="28">
+      <c r="D18" s="23">
         <v>94.8</v>
       </c>
-      <c r="E18" s="28">
+      <c r="E18" s="23">
         <v>32.29</v>
       </c>
-      <c r="F18" s="28">
+      <c r="F18" s="23">
         <v>63.16</v>
       </c>
-      <c r="G18" s="28">
+      <c r="G18" s="23">
         <v>83.55</v>
       </c>
-      <c r="H18" s="28">
+      <c r="H18" s="23">
         <v>73.27</v>
       </c>
-      <c r="I18" s="28">
+      <c r="I18" s="23">
         <v>74.459999999999994</v>
       </c>
-      <c r="J18" s="28">
+      <c r="J18" s="23">
         <v>69.12</v>
       </c>
-      <c r="K18" s="28">
+      <c r="K18" s="23">
         <v>91.62</v>
       </c>
-      <c r="L18" s="28">
+      <c r="L18" s="23">
         <v>75.290000000000006</v>
       </c>
-      <c r="M18" s="28">
+      <c r="M18" s="23">
         <v>63.08</v>
       </c>
       <c r="N18" s="8"/>
@@ -3823,120 +4443,120 @@
       <c r="A19" s="5">
         <v>12</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30"/>
-      <c r="M19" s="30"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
       <c r="N19" s="8"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1">
       <c r="A20" s="5">
         <v>13</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
       <c r="N20" s="8"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1">
       <c r="A21" s="5">
         <v>14</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
       <c r="N21" s="8"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1">
       <c r="A22" s="5">
         <v>15</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="30"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
       <c r="N22" s="8"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1">
       <c r="A23" s="5">
         <v>16</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C23" s="23">
         <v>86.16</v>
       </c>
-      <c r="D23" s="28">
+      <c r="D23" s="23">
         <v>94.8</v>
       </c>
-      <c r="E23" s="28">
+      <c r="E23" s="23">
         <v>32.29</v>
       </c>
-      <c r="F23" s="28">
+      <c r="F23" s="23">
         <v>63.16</v>
       </c>
-      <c r="G23" s="28">
+      <c r="G23" s="23">
         <v>83.55</v>
       </c>
-      <c r="H23" s="28">
+      <c r="H23" s="23">
         <v>73.27</v>
       </c>
-      <c r="I23" s="28">
+      <c r="I23" s="23">
         <v>74.459999999999994</v>
       </c>
-      <c r="J23" s="28">
+      <c r="J23" s="23">
         <v>69.12</v>
       </c>
-      <c r="K23" s="28">
+      <c r="K23" s="23">
         <v>91.62</v>
       </c>
-      <c r="L23" s="28">
+      <c r="L23" s="23">
         <v>75.290000000000006</v>
       </c>
-      <c r="M23" s="28">
+      <c r="M23" s="23">
         <v>63.08</v>
       </c>
       <c r="N23" s="8"/>
@@ -3945,120 +4565,120 @@
       <c r="A24" s="5">
         <v>17</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
       <c r="N24" s="8"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1">
       <c r="A25" s="5">
         <v>18</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
       <c r="N25" s="8"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1">
       <c r="A26" s="5">
         <v>19</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="27"/>
       <c r="N26" s="8"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1">
       <c r="A27" s="5">
         <v>20</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="32"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32"/>
-      <c r="M27" s="32"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="27"/>
       <c r="N27" s="8"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1">
       <c r="A28" s="5">
         <v>21</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="32">
+      <c r="C28" s="27">
         <v>80.87</v>
       </c>
-      <c r="D28" s="32">
+      <c r="D28" s="27">
         <v>95.52</v>
       </c>
-      <c r="E28" s="32">
+      <c r="E28" s="27">
         <v>37.479999999999997</v>
       </c>
-      <c r="F28" s="32">
+      <c r="F28" s="27">
         <v>62.57</v>
       </c>
-      <c r="G28" s="32">
+      <c r="G28" s="27">
         <v>84.87</v>
       </c>
-      <c r="H28" s="32">
+      <c r="H28" s="27">
         <v>72.319999999999993</v>
       </c>
-      <c r="I28" s="32">
+      <c r="I28" s="27">
         <v>70.040000000000006</v>
       </c>
-      <c r="J28" s="32">
+      <c r="J28" s="27">
         <v>63.76</v>
       </c>
-      <c r="K28" s="32">
+      <c r="K28" s="27">
         <v>90.57</v>
       </c>
-      <c r="L28" s="32">
+      <c r="L28" s="27">
         <v>73.349999999999994</v>
       </c>
-      <c r="M28" s="32">
+      <c r="M28" s="27">
         <v>54.65</v>
       </c>
       <c r="N28" s="8"/>
@@ -4067,40 +4687,40 @@
       <c r="A29" s="5">
         <v>22</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="34">
+      <c r="C29" s="29">
         <v>30.14</v>
       </c>
-      <c r="D29" s="34">
+      <c r="D29" s="29">
         <v>58.07</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="29">
         <v>12.89</v>
       </c>
-      <c r="F29" s="34">
+      <c r="F29" s="29">
         <v>29.59</v>
       </c>
-      <c r="G29" s="34">
+      <c r="G29" s="29">
         <v>51</v>
       </c>
-      <c r="H29" s="34">
+      <c r="H29" s="29">
         <v>24.64</v>
       </c>
-      <c r="I29" s="34">
+      <c r="I29" s="29">
         <v>30.13</v>
       </c>
-      <c r="J29" s="34">
+      <c r="J29" s="29">
         <v>32.799999999999997</v>
       </c>
-      <c r="K29" s="34">
+      <c r="K29" s="29">
         <v>70.62</v>
       </c>
-      <c r="L29" s="34">
+      <c r="L29" s="29">
         <v>41.43</v>
       </c>
-      <c r="M29" s="34">
+      <c r="M29" s="29">
         <v>22.07</v>
       </c>
       <c r="N29" s="8"/>
@@ -4109,40 +4729,40 @@
       <c r="A30" s="5">
         <v>23</v>
       </c>
-      <c r="B30" s="33" t="s">
+      <c r="B30" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="34">
+      <c r="C30" s="29">
         <v>43.47</v>
       </c>
-      <c r="D30" s="34">
+      <c r="D30" s="29">
         <v>73.349999999999994</v>
       </c>
-      <c r="E30" s="34">
+      <c r="E30" s="29">
         <v>17.850000000000001</v>
       </c>
-      <c r="F30" s="34">
+      <c r="F30" s="29">
         <v>39.479999999999997</v>
       </c>
-      <c r="G30" s="34">
+      <c r="G30" s="29">
         <v>61.58</v>
       </c>
-      <c r="H30" s="34">
+      <c r="H30" s="29">
         <v>36.53</v>
       </c>
-      <c r="I30" s="34">
+      <c r="I30" s="29">
         <v>42.79</v>
       </c>
-      <c r="J30" s="34">
+      <c r="J30" s="29">
         <v>44.44</v>
       </c>
-      <c r="K30" s="34">
+      <c r="K30" s="29">
         <v>78.72</v>
       </c>
-      <c r="L30" s="34">
+      <c r="L30" s="29">
         <v>53.55</v>
       </c>
-      <c r="M30" s="34">
+      <c r="M30" s="29">
         <v>31.95</v>
       </c>
       <c r="N30" s="8"/>
@@ -4151,40 +4771,40 @@
       <c r="A31" s="5">
         <v>24</v>
       </c>
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="34">
+      <c r="C31" s="29">
         <v>56.35</v>
       </c>
-      <c r="D31" s="34">
+      <c r="D31" s="29">
         <v>84.8</v>
       </c>
-      <c r="E31" s="34">
+      <c r="E31" s="29">
         <v>23.57</v>
       </c>
-      <c r="F31" s="34">
+      <c r="F31" s="29">
         <v>50.06</v>
       </c>
-      <c r="G31" s="34">
+      <c r="G31" s="29">
         <v>68.27</v>
       </c>
-      <c r="H31" s="34">
+      <c r="H31" s="29">
         <v>48.42</v>
       </c>
-      <c r="I31" s="34">
+      <c r="I31" s="29">
         <v>55.15</v>
       </c>
-      <c r="J31" s="34">
+      <c r="J31" s="29">
         <v>54.59</v>
       </c>
-      <c r="K31" s="34">
+      <c r="K31" s="29">
         <v>84.34</v>
       </c>
-      <c r="L31" s="34">
+      <c r="L31" s="29">
         <v>62.23</v>
       </c>
-      <c r="M31" s="34">
+      <c r="M31" s="29">
         <v>41.29</v>
       </c>
       <c r="N31" s="8"/>
@@ -4193,40 +4813,40 @@
       <c r="A32" s="5">
         <v>25</v>
       </c>
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="34">
+      <c r="C32" s="29">
         <v>65.94</v>
       </c>
-      <c r="D32" s="34">
+      <c r="D32" s="29">
         <v>92</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="29">
         <v>29.55</v>
       </c>
-      <c r="F32" s="34">
+      <c r="F32" s="29">
         <v>56.56</v>
       </c>
-      <c r="G32" s="34">
+      <c r="G32" s="29">
         <v>76.930000000000007</v>
       </c>
-      <c r="H32" s="34">
+      <c r="H32" s="29">
         <v>60.82</v>
       </c>
-      <c r="I32" s="34">
+      <c r="I32" s="29">
         <v>63.82</v>
       </c>
-      <c r="J32" s="34">
+      <c r="J32" s="29">
         <v>62.17</v>
       </c>
-      <c r="K32" s="34">
+      <c r="K32" s="29">
         <v>87.78</v>
       </c>
-      <c r="L32" s="34">
+      <c r="L32" s="29">
         <v>69.64</v>
       </c>
-      <c r="M32" s="34">
+      <c r="M32" s="29">
         <v>49.55</v>
       </c>
       <c r="N32" s="8"/>
@@ -4235,40 +4855,40 @@
       <c r="A33" s="5">
         <v>26</v>
       </c>
-      <c r="B33" s="33" t="s">
+      <c r="B33" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="34">
+      <c r="C33" s="29">
         <v>76.42</v>
       </c>
-      <c r="D33" s="34">
+      <c r="D33" s="29">
         <v>94.95</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="29">
         <v>36.39</v>
       </c>
-      <c r="F33" s="34">
+      <c r="F33" s="29">
         <v>63.97</v>
       </c>
-      <c r="G33" s="34">
+      <c r="G33" s="29">
         <v>82.76</v>
       </c>
-      <c r="H33" s="34">
+      <c r="H33" s="29">
         <v>70.08</v>
       </c>
-      <c r="I33" s="34">
+      <c r="I33" s="29">
         <v>70.17</v>
       </c>
-      <c r="J33" s="34">
+      <c r="J33" s="29">
         <v>67.150000000000006</v>
       </c>
-      <c r="K33" s="34">
+      <c r="K33" s="29">
         <v>90.63</v>
       </c>
-      <c r="L33" s="34">
+      <c r="L33" s="29">
         <v>73.72</v>
       </c>
-      <c r="M33" s="34">
+      <c r="M33" s="29">
         <v>55.87</v>
       </c>
       <c r="N33" s="8"/>
@@ -4287,7 +4907,7 @@
     </row>
     <row r="37" spans="1:14" ht="15.75" customHeight="1">
       <c r="A37" s="5"/>
-      <c r="B37" s="19"/>
+      <c r="B37" s="14"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -4303,43 +4923,43 @@
     </row>
     <row r="38" spans="1:14" ht="15.75" customHeight="1">
       <c r="A38" s="5"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="21"/>
-      <c r="L38" s="21"/>
-      <c r="M38" s="21"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
       <c r="N38" s="8"/>
     </row>
     <row r="39" spans="1:14" ht="15.75" customHeight="1">
       <c r="A39" s="5"/>
-      <c r="N39" s="22"/>
+      <c r="N39" s="17"/>
     </row>
     <row r="40" spans="1:14" ht="15.75" customHeight="1">
       <c r="A40" s="5"/>
-      <c r="N40" s="22"/>
+      <c r="N40" s="17"/>
     </row>
     <row r="41" spans="1:14" ht="15.75" customHeight="1">
       <c r="A41" s="5"/>
-      <c r="N41" s="22"/>
+      <c r="N41" s="17"/>
     </row>
     <row r="42" spans="1:14" ht="15.75" customHeight="1">
       <c r="A42" s="5"/>
-      <c r="N42" s="22"/>
+      <c r="N42" s="17"/>
     </row>
     <row r="43" spans="1:14" ht="15.75" customHeight="1">
       <c r="A43" s="5"/>
-      <c r="N43" s="22"/>
+      <c r="N43" s="17"/>
     </row>
     <row r="44" spans="1:14" ht="15.75" customHeight="1">
       <c r="A44" s="5"/>
-      <c r="N44" s="22"/>
+      <c r="N44" s="17"/>
     </row>
     <row r="45" spans="1:14" ht="15.75" customHeight="1">
       <c r="A45" s="5"/>
@@ -4348,34 +4968,34 @@
     <row r="46" spans="1:14" ht="15.75" customHeight="1">
       <c r="A46" s="5"/>
       <c r="B46" s="1"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="24"/>
-      <c r="J46" s="24"/>
-      <c r="K46" s="24"/>
-      <c r="L46" s="24"/>
-      <c r="M46" s="24"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="19"/>
+      <c r="L46" s="19"/>
+      <c r="M46" s="19"/>
       <c r="N46" s="8"/>
     </row>
     <row r="47" spans="1:14" ht="15.75" customHeight="1">
       <c r="A47" s="5"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="21"/>
-      <c r="J47" s="21"/>
-      <c r="K47" s="21"/>
-      <c r="L47" s="21"/>
-      <c r="M47" s="21"/>
-      <c r="N47" s="22"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
+      <c r="M47" s="16"/>
+      <c r="N47" s="17"/>
     </row>
     <row r="48" spans="1:14" ht="15.75" customHeight="1">
       <c r="N48" s="8"/>

</xml_diff>